<commit_message>
New Version with 100% working purchase page
</commit_message>
<xml_diff>
--- a/assets/Copper Price Apr2024.xlsx
+++ b/assets/Copper Price Apr2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcdal\OneDrive\Desktop\LVP Copper\LV-Panels-Copper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BA8E3-F60B-4FA8-ACDD-47723C97A033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D4032A-8A9A-4654-9DD4-C3CFE8F87B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F624A885-E299-461A-B6FC-ACE54AF432D9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F624A885-E299-461A-B6FC-ACE54AF432D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,24 +132,30 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,23 +167,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,7 +510,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -521,384 +538,387 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>177.6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>710.4</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>3.7</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>0.92500000000000004</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2">
-        <v>4670.3999999999996</v>
-      </c>
-      <c r="C3" s="2">
-        <v>18681.599999999999</v>
-      </c>
-      <c r="D3" s="3">
-        <v>97.3</v>
-      </c>
-      <c r="E3" s="3">
-        <v>24.324999999999999</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
+        <v>213.33</v>
+      </c>
+      <c r="C3" s="5">
+        <v>768</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <v>216</v>
+      </c>
+      <c r="C4" s="5">
+        <v>864</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.125</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>364.8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1459.2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>7.6</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
+        <v>522.66999999999996</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1881.6</v>
+      </c>
+      <c r="D6" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2.722</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
+        <v>528</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2112</v>
+      </c>
+      <c r="D7" s="6">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5">
+        <v>688</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2476.8000000000002</v>
+      </c>
+      <c r="D8" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3.5830000000000002</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5">
+        <v>696</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2784</v>
+      </c>
+      <c r="D9" s="6">
+        <v>14.5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5">
+        <v>864</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3456</v>
+      </c>
+      <c r="D10" s="6">
+        <v>18</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" s="7" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1029.33</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3705.6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>19.3</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5.3609999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1173.33</v>
+      </c>
+      <c r="C12" s="5">
+        <v>4224</v>
+      </c>
+      <c r="D12" s="6">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1370.67</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4934.3999999999996</v>
+      </c>
+      <c r="D13" s="6">
+        <v>25.7</v>
+      </c>
+      <c r="E13" s="7">
+        <v>7.1390000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1392</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5568</v>
+      </c>
+      <c r="D14" s="6">
+        <v>29</v>
+      </c>
+      <c r="E14" s="6">
+        <v>7.25</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1728</v>
+      </c>
+      <c r="C15" s="5">
+        <v>6220.8</v>
+      </c>
+      <c r="D15" s="6">
+        <v>32.4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1728</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6912</v>
+      </c>
+      <c r="D16" s="6">
+        <v>36</v>
+      </c>
+      <c r="E16" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2064</v>
+      </c>
+      <c r="C17" s="5">
+        <v>7430.4</v>
+      </c>
+      <c r="D17" s="6">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2075.04</v>
+      </c>
+      <c r="C18" s="5">
+        <v>8300.16</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43.23</v>
+      </c>
+      <c r="E18" s="6">
+        <v>10.807499999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2580</v>
+      </c>
+      <c r="C19" s="5">
+        <v>9288</v>
+      </c>
+      <c r="D19" s="6">
+        <v>48.38</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2592</v>
+      </c>
+      <c r="C20" s="5">
+        <v>10368</v>
+      </c>
+      <c r="D20" s="6">
+        <v>54</v>
+      </c>
+      <c r="E20" s="6">
+        <v>13.5</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B21" s="5">
         <v>2752</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C21" s="5">
         <v>9907.2000000000007</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D21" s="6">
         <v>51.6</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B22" s="2">
         <v>3096</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C22" s="2">
         <v>12384</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D22" s="3">
         <v>64.5</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E22" s="3">
         <v>16.125</v>
       </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2580</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9288</v>
-      </c>
-      <c r="D6" s="3">
-        <v>48.38</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2592</v>
-      </c>
-      <c r="C7" s="2">
-        <v>10368</v>
-      </c>
-      <c r="D7" s="3">
-        <v>54</v>
-      </c>
-      <c r="E7" s="3">
-        <v>13.5</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2064</v>
-      </c>
-      <c r="C8" s="2">
-        <v>7430.4</v>
-      </c>
-      <c r="D8" s="3">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2075.04</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8300.16</v>
-      </c>
-      <c r="D9" s="3">
-        <v>43.23</v>
-      </c>
-      <c r="E9" s="3">
-        <v>10.807499999999999</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1728</v>
-      </c>
-      <c r="C10" s="2">
-        <v>6220.8</v>
-      </c>
-      <c r="D10" s="3">
-        <v>32.4</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1728</v>
-      </c>
-      <c r="C11" s="2">
-        <v>6912</v>
-      </c>
-      <c r="D11" s="3">
-        <v>36</v>
-      </c>
-      <c r="E11" s="3">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1370.67</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4934.3999999999996</v>
-      </c>
-      <c r="D12" s="3">
-        <v>25.7</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1392</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5568</v>
-      </c>
-      <c r="D13" s="3">
-        <v>29</v>
-      </c>
-      <c r="E13" s="3">
-        <v>7.25</v>
-      </c>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1029.33</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3705.6</v>
-      </c>
-      <c r="D14" s="3">
-        <v>19.3</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1173.33</v>
-      </c>
-      <c r="C15" s="2">
-        <v>4224</v>
-      </c>
-      <c r="D15" s="3">
-        <v>22</v>
-      </c>
-      <c r="E15" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
-        <v>864</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3456</v>
-      </c>
-      <c r="D16" s="3">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
-        <v>688</v>
-      </c>
-      <c r="C17" s="2">
-        <v>2476.8000000000002</v>
-      </c>
-      <c r="D17" s="3">
-        <v>12.9</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
-        <v>696</v>
-      </c>
-      <c r="C18" s="2">
-        <v>2784</v>
-      </c>
-      <c r="D18" s="3">
-        <v>14.5</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3.625</v>
-      </c>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2">
-        <v>522.66999999999996</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1881.6</v>
-      </c>
-      <c r="D19" s="3">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2">
-        <v>528</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2112</v>
-      </c>
-      <c r="D20" s="3">
-        <v>11</v>
-      </c>
-      <c r="E20" s="3">
-        <v>2.75</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2">
-        <v>364.8</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1459.2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2">
-        <v>213.33</v>
-      </c>
-      <c r="C22" s="2">
-        <v>768</v>
-      </c>
-      <c r="D22" s="3">
-        <v>4</v>
-      </c>
-      <c r="E22" s="4"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="2">
-        <v>216</v>
+        <v>4670.3999999999996</v>
       </c>
       <c r="C23" s="2">
-        <v>864</v>
+        <v>18681.599999999999</v>
       </c>
       <c r="D23" s="3">
-        <v>4.5</v>
+        <v>97.3</v>
       </c>
       <c r="E23" s="3">
-        <v>1.125</v>
+        <v>24.324999999999999</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+    <sortCondition ref="B1:B25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>